<commit_message>
Load and preprocess IJC (7/17 release)
</commit_message>
<xml_diff>
--- a/raw/ijc_710.xlsx
+++ b/raw/ijc_710.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwong\Documents\verition-summer-2025\Verition\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E4E4FCF-3366-4264-B401-44FD25348AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E604403-7C6A-4158-BC20-7D203EBC3B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="-21720" windowWidth="38640" windowHeight="21120"/>
+    <workbookView xWindow="4875" yWindow="4740" windowWidth="28800" windowHeight="15345"/>
   </bookViews>
   <sheets>
     <sheet name="Book1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
   <si>
     <t>INJCJC Index</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Actual</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
     <t>Prior</t>
   </si>
   <si>
@@ -76,7 +73,7 @@
     <t>Average Estimate</t>
   </si>
   <si>
-    <t>235.17k</t>
+    <t>235.20k</t>
   </si>
   <si>
     <t>High Estimate</t>
@@ -100,7 +97,7 @@
     <t>Standard Deviation</t>
   </si>
   <si>
-    <t>4.97k</t>
+    <t>4.96k</t>
   </si>
   <si>
     <t>Custom Estimate</t>
@@ -154,9 +151,6 @@
     <t>Citigroup Inc</t>
   </si>
   <si>
-    <t>7th</t>
-  </si>
-  <si>
     <t>William Adams</t>
   </si>
   <si>
@@ -331,16 +325,13 @@
     <t>Herrmann Forecasting LLC</t>
   </si>
   <si>
-    <t>7/08/2025</t>
+    <t>7/09/2025</t>
   </si>
   <si>
     <t>2nd</t>
   </si>
   <si>
     <t>Bloomberg Economics</t>
-  </si>
-  <si>
-    <t>7/09/2025</t>
   </si>
 </sst>
 </file>
@@ -1275,8 +1266,8 @@
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
+      <c r="C7" s="1">
+        <v>227</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1285,7 +1276,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>233</v>
@@ -1297,10 +1288,10 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
+        <v>232</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1316,7 +1307,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1327,10 +1318,10 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1339,10 +1330,10 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1351,10 +1342,10 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1363,10 +1354,10 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1375,7 +1366,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1">
         <v>37</v>
@@ -1387,10 +1378,10 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1399,10 +1390,10 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1411,7 +1402,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1428,7 +1419,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1439,68 +1430,68 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D23" s="1">
         <v>240</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D24" s="1">
         <v>239</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D25" s="1">
         <v>235</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -1508,13 +1499,13 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="1">
         <v>242</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -1522,207 +1513,205 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1">
         <v>228</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D28" s="1">
         <v>245</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D29" s="1">
         <v>237</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D30" s="1">
         <v>238</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D31" s="1">
         <v>240</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D32" s="1">
         <v>237</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D33" s="1">
         <v>235</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D34" s="1">
         <v>243</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D35" s="1">
         <v>235</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D36" s="1">
         <v>245</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37" s="1">
         <v>230</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D38" s="1">
         <v>225</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D39" s="1">
         <v>230</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F39" s="1"/>
     </row>
@@ -1730,13 +1719,13 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D40" s="1">
         <v>234</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F40" s="1"/>
     </row>
@@ -1744,13 +1733,13 @@
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D41" s="1">
         <v>235</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F41" s="1"/>
     </row>
@@ -1758,29 +1747,29 @@
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D42" s="1">
         <v>230</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D43" s="1">
         <v>240</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F43" s="1"/>
     </row>
@@ -1788,161 +1777,161 @@
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D44" s="1">
         <v>230</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D45" s="1">
         <v>235</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D46" s="1">
         <v>234</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D47" s="1">
         <v>235</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D48" s="1">
         <v>236</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D49" s="1">
         <v>225</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D50" s="1">
         <v>235</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D51" s="1">
         <v>234</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D52" s="1">
         <v>235</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D53" s="1">
         <v>235</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F53" s="1"/>
     </row>
@@ -1950,29 +1939,29 @@
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D54" s="1">
         <v>235</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D55" s="1">
         <v>240</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F55" s="1"/>
     </row>
@@ -1980,61 +1969,61 @@
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D56" s="1">
         <v>240</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D57" s="1">
         <v>228</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D58" s="1">
+        <v>233</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="D58" s="1">
-        <v>232</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D59" s="1">
         <v>229</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F59" s="1"/>
     </row>

</xml_diff>